<commit_message>
auto:modifying the SRQ form
</commit_message>
<xml_diff>
--- a/config/forms/app/srq.xlsx
+++ b/config/forms/app/srq.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -60,91 +60,52 @@
     <t>person</t>
   </si>
   <si>
-    <t>Person Completing the Questionarie</t>
+    <t>Name of Person Completing Questionnaire</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Date SRQ Completed</t>
+  </si>
+  <si>
+    <t>vl_results</t>
+  </si>
+  <si>
+    <t>Viral Load Results:</t>
+  </si>
+  <si>
+    <t>cd4_results</t>
+  </si>
+  <si>
+    <t>CD4 Results</t>
+  </si>
+  <si>
+    <t>vl_date</t>
+  </si>
+  <si>
+    <t>Most recent VL test date:</t>
+  </si>
+  <si>
+    <t>vl_cd4</t>
+  </si>
+  <si>
+    <t>Most recent CD4 test date:</t>
+  </si>
+  <si>
+    <t>regime</t>
+  </si>
+  <si>
+    <t>Current ART Regime:</t>
+  </si>
+  <si>
+    <t>regime_date</t>
+  </si>
+  <si>
+    <t>Date Regime started:</t>
   </si>
   <si>
     <t xml:space="preserve">end group </t>
-  </si>
-  <si>
-    <t>treatment_inputs</t>
-  </si>
-  <si>
-    <t>Adherence Questionarie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string </t>
-  </si>
-  <si>
-    <t>client_name</t>
-  </si>
-  <si>
-    <t>Client Name:</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>tel</t>
-  </si>
-  <si>
-    <t>telephone</t>
-  </si>
-  <si>
-    <t>Telephone number</t>
-  </si>
-  <si>
-    <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>docket</t>
-  </si>
-  <si>
-    <t>Docket number</t>
-  </si>
-  <si>
-    <t>vl_results</t>
-  </si>
-  <si>
-    <t>VL Results:</t>
-  </si>
-  <si>
-    <t>cd4_results</t>
-  </si>
-  <si>
-    <t>CD4 Results</t>
-  </si>
-  <si>
-    <t>vl_date</t>
-  </si>
-  <si>
-    <t>Most recent VL test date:</t>
-  </si>
-  <si>
-    <t>vl_cd4</t>
-  </si>
-  <si>
-    <t>Most recent CD4 test date:</t>
-  </si>
-  <si>
-    <t>regime</t>
-  </si>
-  <si>
-    <t>Current ART Regime:</t>
-  </si>
-  <si>
-    <t>regime_date</t>
-  </si>
-  <si>
-    <t>Date Regime started:</t>
   </si>
   <si>
     <t>cd4</t>
@@ -218,6 +179,15 @@
 or No</t>
   </si>
   <si>
+    <t>select_one pill</t>
+  </si>
+  <si>
+    <t>pills</t>
+  </si>
+  <si>
+    <t>Was pill-count done?</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -392,10 +362,22 @@
     <t>Stressed out</t>
   </si>
   <si>
-    <t>pills</t>
-  </si>
-  <si>
     <t>Tired of taking pills</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>form_title</t>
@@ -432,7 +414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -464,11 +446,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -480,7 +457,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +468,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -520,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -545,16 +516,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -868,32 +833,32 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>22</v>
@@ -901,240 +866,181 @@
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="I8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0.0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="4"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
+      <c r="A12" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" ht="26.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" ht="60.75" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="4"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+        <v>51</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" ht="26.25" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" ht="60.75" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="5"/>
+      <c r="A25" s="5"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1156,7 +1062,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1167,332 +1073,354 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1512,43 +1440,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>130</v>
+        <v>121</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="12">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G2" s="3"/>
     </row>

</xml_diff>

<commit_message>
auto:modifications in the srq form
</commit_message>
<xml_diff>
--- a/config/forms/app/srq.xlsx
+++ b/config/forms/app/srq.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
   <si>
     <t>type</t>
   </si>
@@ -45,7 +45,7 @@
     <t>begin group</t>
   </si>
   <si>
-    <t>srq</t>
+    <t>cd4</t>
   </si>
   <si>
     <t>NO_LABEL</t>
@@ -67,48 +67,6 @@
   </si>
   <si>
     <t>Date SRQ Completed</t>
-  </si>
-  <si>
-    <t>vl_results</t>
-  </si>
-  <si>
-    <t>Viral Load Results:</t>
-  </si>
-  <si>
-    <t>cd4_results</t>
-  </si>
-  <si>
-    <t>CD4 Results</t>
-  </si>
-  <si>
-    <t>vl_date</t>
-  </si>
-  <si>
-    <t>Most recent VL test date:</t>
-  </si>
-  <si>
-    <t>vl_cd4</t>
-  </si>
-  <si>
-    <t>Most recent CD4 test date:</t>
-  </si>
-  <si>
-    <t>regime</t>
-  </si>
-  <si>
-    <t>Current ART Regime:</t>
-  </si>
-  <si>
-    <t>regime_date</t>
-  </si>
-  <si>
-    <t>Date Regime started:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group </t>
-  </si>
-  <si>
-    <t>cd4</t>
   </si>
   <si>
     <t>note</t>
@@ -188,6 +146,9 @@
     <t>Was pill-count done?</t>
   </si>
   <si>
+    <t xml:space="preserve">end group </t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -398,7 +359,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>SRQ FORM</t>
+    <t xml:space="preserve">Form - SRQ </t>
+  </si>
+  <si>
+    <t>srq</t>
   </si>
   <si>
     <t>pages</t>
@@ -414,7 +378,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -444,12 +408,6 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -491,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -516,10 +474,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -834,213 +789,121 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" ht="26.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" ht="60.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
+      <c r="A12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
+        <v>39</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" ht="26.25" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18" ht="60.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="5"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="5"/>
+      <c r="A20" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1062,7 +925,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1073,354 +936,354 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1440,43 +1303,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>124</v>
+        <v>108</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="12">
+        <v>113</v>
+      </c>
+      <c r="C2" s="11">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G2" s="3"/>
     </row>

</xml_diff>

<commit_message>
auto:add patient identifier card in the srq form
</commit_message>
<xml_diff>
--- a/config/forms/app/srq.xlsx
+++ b/config/forms/app/srq.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="193">
   <si>
     <t>type</t>
   </si>
@@ -93,6 +93,21 @@
     <t>patient_id</t>
   </si>
   <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>person</t>
   </si>
   <si>
@@ -198,10 +213,119 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>patient_name1</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name1</t>
+  </si>
+  <si>
+    <t>patient_aka</t>
+  </si>
+  <si>
+    <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
+  </si>
+  <si>
+    <t>patient_date_of_birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth </t>
+  </si>
+  <si>
+    <t>../inputs/contact/date_of_birth</t>
+  </si>
+  <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)</t>
+  </si>
+  <si>
+    <t>last_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/lstname != '', instance('contact-summary')/context/lstname, .)</t>
+  </si>
+  <si>
+    <t>date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
+  </si>
+  <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>cd4</t>
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 yellow </t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>note_one</t>
@@ -581,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -622,6 +746,12 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -637,11 +767,14 @@
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1041,409 +1174,1169 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
+      <c r="B16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="4"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="G18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="C24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19"/>
-      <c r="X24" s="19"/>
-      <c r="Y24" s="19"/>
-      <c r="Z24" s="19"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="C29" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="21"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="21"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="21"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="21"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="23"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="15"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
+      <c r="Z46" s="15"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="15"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="15"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" ht="26.25" customHeight="1">
+      <c r="A53" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J53" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" ht="60.75" customHeight="1">
+      <c r="A54" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="F54" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" ht="26.25" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" ht="60.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="F32" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="5"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="5"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
+    </row>
     <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="5"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
     <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="5"/>
+    </row>
     <row r="61" ht="15.75" customHeight="1"/>
     <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="5"/>
+    </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -2390,6 +3283,28 @@
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
+    <row r="1020" ht="15.75" customHeight="1"/>
+    <row r="1021" ht="15.75" customHeight="1"/>
+    <row r="1022" ht="15.75" customHeight="1"/>
+    <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
+    <row r="1030" ht="15.75" customHeight="1"/>
+    <row r="1031" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2412,7 +3327,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2423,332 +3338,332 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
@@ -3740,43 +4655,43 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>146</v>
+        <v>184</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>187</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="25">
+        <v>189</v>
+      </c>
+      <c r="C2" s="28">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="G2" s="3"/>
     </row>

</xml_diff>